<commit_message>
added RMSE to excel file
</commit_message>
<xml_diff>
--- a/Lab1/dat/Weight-Height data.xlsx
+++ b/Lab1/dat/Weight-Height data.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616F57D6-225B-42CE-A31F-B7B28EC2B9D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H3" authorId="0">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -157,8 +168,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>H</t>
   </si>
@@ -189,12 +222,15 @@
   <si>
     <t>H-100=y</t>
   </si>
+  <si>
+    <t>RMSE:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,8 +251,16 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +270,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -304,12 +354,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -356,7 +416,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,9 +448,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,6 +500,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -597,14 +693,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
@@ -612,7 +708,7 @@
     <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -640,8 +736,15 @@
       <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="M1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="8" cm="1">
+        <f t="array" ref="N1">SQRT(SUMSQ(J3:J19-I3:I19) / COUNTA(J3:J19))</f>
+        <v>15.867408358940054</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -671,7 +774,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>6</v>
       </c>
@@ -691,22 +794,22 @@
       </c>
       <c r="H3" s="3">
         <f>CONVERT(E3,"in","cm")</f>
-        <v>187.96</v>
+        <v>187.95999999999998</v>
       </c>
       <c r="I3" s="3">
         <f>CONVERT(F3,"lbm","kg")</f>
-        <v>138.3456544733875</v>
+        <v>138.34567285</v>
       </c>
       <c r="J3" s="3">
         <f>H3-100</f>
-        <v>87.960000000000008</v>
+        <v>87.95999999999998</v>
       </c>
       <c r="K3" s="3">
         <f>I3-J3</f>
-        <v>50.38565447338749</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>50.38567285000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>5</v>
       </c>
@@ -730,7 +833,7 @@
       </c>
       <c r="I4" s="3">
         <f t="shared" ref="I4:I19" si="3">CONVERT(F4,"lbm","kg")</f>
-        <v>90.264869640013487</v>
+        <v>90.264881630000005</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ref="J4:J19" si="4">H4-100</f>
@@ -738,10 +841,10 @@
       </c>
       <c r="K4" s="3">
         <f t="shared" ref="K4:K19" si="5">I4-J4</f>
-        <v>12.464869640013475</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>12.464881629999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -765,7 +868,7 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" si="3"/>
-        <v>83.914577303530123</v>
+        <v>83.914588450000011</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" si="4"/>
@@ -773,10 +876,10 @@
       </c>
       <c r="K5" s="3">
         <f t="shared" si="5"/>
-        <v>8.6545773035301323</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>8.6545884500000199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -800,7 +903,7 @@
       </c>
       <c r="I6" s="3">
         <f t="shared" si="3"/>
-        <v>61.234961816089552</v>
+        <v>61.23496995</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="4"/>
@@ -808,10 +911,10 @@
       </c>
       <c r="K6" s="3">
         <f t="shared" si="5"/>
-        <v>1.2149618160895415</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>1.2149699499999898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -835,7 +938,7 @@
       </c>
       <c r="I7" s="3">
         <f t="shared" si="3"/>
-        <v>58.96700026734549</v>
+        <v>58.967008100000001</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="4"/>
@@ -843,10 +946,10 @@
       </c>
       <c r="K7" s="3">
         <f t="shared" si="5"/>
-        <v>-3.592999732654512</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>-3.5929919000000012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -870,7 +973,7 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" si="3"/>
-        <v>95.254385047250423</v>
+        <v>95.254397699999998</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="4"/>
@@ -878,10 +981,10 @@
       </c>
       <c r="K8" s="3">
         <f t="shared" si="5"/>
-        <v>22.534385047250424</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>22.5343977</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -901,22 +1004,22 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" si="2"/>
-        <v>185.42</v>
+        <v>185.42000000000002</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="3"/>
-        <v>87.089723471771805</v>
+        <v>87.089735040000008</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="4"/>
-        <v>85.419999999999987</v>
+        <v>85.420000000000016</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" si="5"/>
-        <v>1.6697234717718175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>1.669735039999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>5</v>
       </c>
@@ -940,7 +1043,7 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" si="3"/>
-        <v>86.182538852274192</v>
+        <v>86.182550300000003</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="4"/>
@@ -948,10 +1051,10 @@
       </c>
       <c r="K10" s="3">
         <f t="shared" si="5"/>
-        <v>10.922538852274201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>10.922550300000012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -975,7 +1078,7 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" si="3"/>
-        <v>83.914577303530123</v>
+        <v>83.914588450000011</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="4"/>
@@ -983,10 +1086,10 @@
       </c>
       <c r="K11" s="3">
         <f t="shared" si="5"/>
-        <v>8.6545773035301323</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>8.6545884500000199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>5</v>
       </c>
@@ -1010,7 +1113,7 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" si="3"/>
-        <v>72.574769559809837</v>
+        <v>72.574779200000009</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="4"/>
@@ -1018,10 +1121,10 @@
       </c>
       <c r="K12" s="3">
         <f t="shared" si="5"/>
-        <v>-2.6852304401901534</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>-2.685220799999982</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>6</v>
       </c>
@@ -1045,7 +1148,7 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" si="3"/>
-        <v>74.842731108553906</v>
+        <v>74.842741050000001</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="4"/>
@@ -1053,10 +1156,10 @@
       </c>
       <c r="K13" s="3">
         <f t="shared" si="5"/>
-        <v>-8.0372688914460895</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>-8.0372589499999947</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>6</v>
       </c>
@@ -1080,7 +1183,7 @@
       </c>
       <c r="I14" s="3">
         <f t="shared" si="3"/>
-        <v>81.646615754786069</v>
+        <v>81.646626600000005</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="4"/>
@@ -1088,10 +1191,10 @@
       </c>
       <c r="K14" s="3">
         <f t="shared" si="5"/>
-        <v>-1.2333842452139265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>-1.2333733999999907</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -1115,7 +1218,7 @@
       </c>
       <c r="I15" s="3">
         <f t="shared" si="3"/>
-        <v>95.254385047250423</v>
+        <v>95.254397699999998</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="4"/>
@@ -1123,10 +1226,10 @@
       </c>
       <c r="K15" s="3">
         <f t="shared" si="5"/>
-        <v>19.994385047250432</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>19.994397700000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>6</v>
       </c>
@@ -1146,22 +1249,22 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" si="2"/>
-        <v>185.42</v>
+        <v>185.42000000000002</v>
       </c>
       <c r="I16" s="3">
         <f t="shared" si="3"/>
-        <v>86.182538852274192</v>
+        <v>86.182550300000003</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" si="4"/>
-        <v>85.419999999999987</v>
+        <v>85.420000000000016</v>
       </c>
       <c r="K16" s="3">
         <f t="shared" si="5"/>
-        <v>0.76253885227420426</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>0.76255029999998669</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>5</v>
       </c>
@@ -1185,7 +1288,7 @@
       </c>
       <c r="I17" s="3">
         <f t="shared" si="3"/>
-        <v>49.895154072369259</v>
+        <v>49.895160699999998</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="4"/>
@@ -1193,10 +1296,10 @@
       </c>
       <c r="K17" s="3">
         <f t="shared" si="5"/>
-        <v>-10.124845927630751</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>-10.124839300000012</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>5</v>
       </c>
@@ -1220,7 +1323,7 @@
       </c>
       <c r="I18" s="3">
         <f t="shared" si="3"/>
-        <v>54.431077169857375</v>
+        <v>54.431084400000003</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" si="4"/>
@@ -1228,10 +1331,10 @@
       </c>
       <c r="K18" s="3">
         <f t="shared" si="5"/>
-        <v>-3.0489228301426152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>-3.0489155999999866</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>6</v>
       </c>
@@ -1251,19 +1354,19 @@
       </c>
       <c r="H19" s="3">
         <f t="shared" si="2"/>
-        <v>185.42</v>
+        <v>185.42000000000002</v>
       </c>
       <c r="I19" s="3">
         <f t="shared" si="3"/>
-        <v>99.790308144738518</v>
+        <v>99.790321399999996</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" si="4"/>
-        <v>85.419999999999987</v>
+        <v>85.420000000000016</v>
       </c>
       <c r="K19" s="3">
         <f t="shared" si="5"/>
-        <v>14.37030814473853</v>
+        <v>14.37032139999998</v>
       </c>
     </row>
   </sheetData>
@@ -1274,24 +1377,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>